<commit_message>
output file V1 done and other in progress
</commit_message>
<xml_diff>
--- a/Opt_X.xlsx
+++ b/Opt_X.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mathias/P2X/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rolvur Reinert\Desktop\P2X\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C480F746-B6DF-8E4B-9148-7E6F8A410F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D635D562-FB52-4D55-9FA2-B5C5E3086996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="460" windowWidth="25340" windowHeight="14700" xr2:uid="{AF05AB96-9D53-9746-847A-2DA4A160AAD8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AF05AB96-9D53-9746-847A-2DA4A160AAD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Run" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="138">
   <si>
     <t>First day of the simulation</t>
   </si>
@@ -442,12 +442,6 @@
     <t>S_Pu_max</t>
   </si>
   <si>
-    <t>2020-01-06 00:00</t>
-  </si>
-  <si>
-    <t>2020-01-12 23:59</t>
-  </si>
-  <si>
     <t>2020-01-13 00:00</t>
   </si>
   <si>
@@ -455,6 +449,9 @@
   </si>
   <si>
     <t>Weekly</t>
+  </si>
+  <si>
+    <t>2020-01-26 23:59</t>
   </si>
 </sst>
 </file>
@@ -961,18 +958,18 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.69921875" customWidth="1"/>
+    <col min="2" max="2" width="39.69921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="70" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -986,18 +983,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>110</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -1014,12 +1011,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>78</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1031,12 +1028,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1048,12 +1045,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -1065,12 +1062,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -1082,7 +1079,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>117</v>
       </c>
@@ -1090,7 +1087,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1107,7 +1104,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1118,7 +1115,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>121</v>
       </c>
@@ -1135,7 +1132,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>120</v>
       </c>
@@ -1146,7 +1143,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>122</v>
       </c>
@@ -1160,7 +1157,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
@@ -1174,7 +1171,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -1185,7 +1182,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
@@ -1196,7 +1193,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
@@ -1207,14 +1204,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>31</v>
       </c>
@@ -1222,7 +1219,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>32</v>
       </c>
@@ -1230,7 +1227,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>33</v>
       </c>
@@ -1238,7 +1235,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
         <v>34</v>
       </c>
@@ -1246,7 +1243,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
         <v>81</v>
       </c>
@@ -1254,7 +1251,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
         <v>83</v>
       </c>
@@ -1262,7 +1259,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
         <v>84</v>
       </c>
@@ -1270,7 +1267,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
         <v>85</v>
       </c>
@@ -1278,7 +1275,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>86</v>
       </c>
@@ -1286,7 +1283,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>87</v>
       </c>
@@ -1294,7 +1291,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
         <v>100</v>
       </c>
@@ -1302,7 +1299,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
         <v>95</v>
       </c>
@@ -1310,7 +1307,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="18" t="s">
         <v>96</v>
       </c>
@@ -1318,7 +1315,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
         <v>97</v>
       </c>
@@ -1326,7 +1323,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="18" t="s">
         <v>98</v>
       </c>
@@ -1334,7 +1331,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="18" t="s">
         <v>99</v>
       </c>
@@ -1342,7 +1339,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="18" t="s">
         <v>112</v>
       </c>
@@ -1350,7 +1347,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="18" t="s">
         <v>115</v>
       </c>
@@ -1358,7 +1355,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="18" t="s">
         <v>116</v>
       </c>
@@ -1366,7 +1363,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="18" t="s">
         <v>104</v>
       </c>
@@ -1374,7 +1371,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="18" t="s">
         <v>108</v>
       </c>
@@ -1382,7 +1379,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="18" t="s">
         <v>109</v>
       </c>
@@ -1426,18 +1423,18 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="85" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.19921875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -1448,7 +1445,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>36</v>
       </c>
@@ -1467,7 +1464,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>37</v>
       </c>
@@ -1489,7 +1486,7 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>38</v>
       </c>
@@ -1508,7 +1505,7 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>39</v>
       </c>
@@ -1527,7 +1524,7 @@
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>40</v>
       </c>
@@ -1546,7 +1543,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>41</v>
       </c>
@@ -1565,7 +1562,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>42</v>
       </c>
@@ -1584,7 +1581,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
         <v>13</v>
       </c>
@@ -1608,7 +1605,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>61</v>
       </c>
@@ -1628,7 +1625,7 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>63</v>
       </c>
@@ -1647,7 +1644,7 @@
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>43</v>
       </c>
@@ -1666,7 +1663,7 @@
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>123</v>
       </c>
@@ -1683,7 +1680,7 @@
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>133</v>
       </c>
@@ -1700,7 +1697,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>45</v>
       </c>
@@ -1717,7 +1714,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>47</v>
       </c>
@@ -1733,7 +1730,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>50</v>
       </c>
@@ -1750,7 +1747,7 @@
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>44</v>
       </c>
@@ -1767,7 +1764,7 @@
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>46</v>
       </c>
@@ -1784,7 +1781,7 @@
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>49</v>
       </c>
@@ -1801,7 +1798,7 @@
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -1818,7 +1815,7 @@
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>48</v>
       </c>
@@ -1835,7 +1832,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>51</v>
       </c>
@@ -1852,7 +1849,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>52</v>
       </c>
@@ -1871,7 +1868,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>53</v>
       </c>
@@ -1890,7 +1887,7 @@
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
@@ -1898,7 +1895,7 @@
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
@@ -1906,7 +1903,7 @@
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
@@ -1914,7 +1911,7 @@
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
@@ -1922,7 +1919,7 @@
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
@@ -1930,7 +1927,7 @@
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
@@ -1938,7 +1935,7 @@
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
@@ -1946,7 +1943,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
@@ -1954,7 +1951,7 @@
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
@@ -1962,7 +1959,7 @@
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
@@ -1970,7 +1967,7 @@
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
@@ -1978,7 +1975,7 @@
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
@@ -1986,7 +1983,7 @@
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="11"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -1997,7 +1994,7 @@
       <c r="H38" s="11"/>
       <c r="I38" s="11"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -2008,7 +2005,7 @@
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -2019,7 +2016,7 @@
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="11"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -2030,7 +2027,7 @@
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="11"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -2041,7 +2038,7 @@
       <c r="H42" s="11"/>
       <c r="I42" s="11"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="11"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -2052,7 +2049,7 @@
       <c r="H43" s="11"/>
       <c r="I43" s="11"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -2063,7 +2060,7 @@
       <c r="H44" s="11"/>
       <c r="I44" s="11"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -2074,7 +2071,7 @@
       <c r="H45" s="11"/>
       <c r="I45" s="11"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="11"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -2101,9 +2098,9 @@
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>101</v>
       </c>
@@ -2111,7 +2108,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="20">
         <v>1.0000000000000001E-5</v>
       </c>
@@ -2119,7 +2116,7 @@
         <v>2.3193049701884466E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -2127,7 +2124,7 @@
         <v>23.104209695952736</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <v>2</v>
       </c>
@@ -2135,7 +2132,7 @@
         <v>46.032093621114697</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="20">
         <v>3</v>
       </c>
@@ -2143,7 +2140,7 @@
         <v>68.785662616162213</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="20">
         <v>4</v>
       </c>
@@ -2151,7 +2148,7 @@
         <v>91.366897061730668</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="20">
         <v>5</v>
       </c>
@@ -2159,7 +2156,7 @@
         <v>113.77774745299608</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="20">
         <v>6</v>
       </c>
@@ -2167,7 +2164,7 @@
         <v>136.02013496129942</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="20">
         <v>7</v>
       </c>
@@ -2175,7 +2172,7 @@
         <v>158.09595198315293</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="20">
         <v>8</v>
       </c>
@@ -2183,7 +2180,7 @@
         <v>180.00706267695841</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="20">
         <v>9</v>
       </c>
@@ -2191,7 +2188,7 @@
         <v>201.75530348775646</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="20">
         <v>10</v>
       </c>
@@ -2199,7 +2196,7 @@
         <v>223.34248366031795</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="20">
         <v>11</v>
       </c>
@@ -2207,7 +2204,7 @@
         <v>244.77038574087737</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="20">
         <v>12</v>
       </c>
@@ -2215,7 +2212,7 @@
         <v>266.04076606780194</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="20">
         <v>13</v>
       </c>
@@ -2223,7 +2220,7 @@
         <v>287.15535525147862</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="20">
         <v>14</v>
       </c>
@@ -2231,7 +2228,7 @@
         <v>308.11585864369528</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="20">
         <v>15</v>
       </c>
@@ -2239,7 +2236,7 @@
         <v>328.9239567967831</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="20">
         <v>16</v>
       </c>
@@ -2247,7 +2244,7 @@
         <v>349.58130591278024</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="20">
         <v>17</v>
       </c>
@@ -2255,7 +2252,7 @@
         <v>370.08953828286798</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="20">
         <v>18</v>
       </c>
@@ -2263,7 +2260,7 @@
         <v>390.45026271732496</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="20">
         <v>19</v>
       </c>
@@ -2271,7 +2268,7 @@
         <v>410.66506496623748</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="20">
         <v>20</v>
       </c>
@@ -2279,7 +2276,7 @@
         <v>430.73550813119624</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="20">
         <v>21</v>
       </c>
@@ -2287,7 +2284,7 @@
         <v>450.66313306820444</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="20">
         <v>22</v>
       </c>
@@ -2295,7 +2292,7 @@
         <v>470.44945878201548</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="20">
         <v>23</v>
       </c>
@@ -2303,7 +2300,7 @@
         <v>490.09598281211152</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="20">
         <v>24</v>
       </c>
@@ -2311,7 +2308,7 @@
         <v>509.60418161053019</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="20">
         <v>25</v>
       </c>
@@ -2319,7 +2316,7 @@
         <v>528.97551091173773</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="20">
         <v>26</v>
       </c>
@@ -2327,7 +2324,7 @@
         <v>548.21140609474503</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="20">
         <v>27</v>
       </c>
@@ -2335,7 +2332,7 @@
         <v>567.31328253765537</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="20">
         <v>28</v>
       </c>
@@ -2343,7 +2340,7 @@
         <v>586.28253596482523</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="20">
         <v>29</v>
       </c>
@@ -2351,7 +2348,7 @@
         <v>605.12054278682263</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="20">
         <v>30</v>
       </c>
@@ -2359,7 +2356,7 @@
         <v>623.82866043334957</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="20">
         <v>31</v>
       </c>
@@ -2367,7 +2364,7 @@
         <v>642.40822767930479</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="20">
         <v>32</v>
       </c>
@@ -2375,7 +2372,7 @@
         <v>660.86056496414619</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="20">
         <v>33</v>
       </c>
@@ -2383,7 +2380,7 @@
         <v>679.18697470471477</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="20">
         <v>34</v>
       </c>
@@ -2391,7 +2388,7 @@
         <v>697.38874160167734</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="20">
         <v>35</v>
       </c>
@@ -2399,7 +2396,7 @@
         <v>715.46713293973596</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="20">
         <v>36</v>
       </c>
@@ -2407,7 +2404,7 @@
         <v>733.42339888175422</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="20">
         <v>37</v>
       </c>
@@ -2415,7 +2412,7 @@
         <v>751.25877275694381</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="20">
         <v>38</v>
       </c>
@@ -2423,7 +2420,7 @@
         <v>768.97447134324705</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="20">
         <v>39</v>
       </c>
@@ -2431,7 +2428,7 @@
         <v>786.57169514405768</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="20">
         <v>40</v>
       </c>
@@ -2439,7 +2436,7 @@
         <v>804.0516286594052</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="20">
         <v>41</v>
       </c>
@@ -2447,7 +2444,7 @@
         <v>821.41544065173696</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="20">
         <v>42</v>
       </c>
@@ -2455,7 +2452,7 @@
         <v>838.66428440641982</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="20">
         <v>43</v>
       </c>
@@ -2463,7 +2460,7 @@
         <v>855.79929798708417</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="20">
         <v>44</v>
       </c>
@@ -2471,7 +2468,7 @@
         <v>872.82160448593072</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="20">
         <v>45</v>
       </c>
@@ -2479,7 +2476,7 @@
         <v>889.73231226911184</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="20">
         <v>46</v>
       </c>
@@ -2487,7 +2484,7 @@
         <v>906.53251521730544</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="20">
         <v>47</v>
       </c>
@@ -2495,7 +2492,7 @@
         <v>923.22329296158534</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="20">
         <v>48</v>
       </c>
@@ -2503,7 +2500,7 @@
         <v>939.80571111469987</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="20">
         <v>49</v>
       </c>
@@ -2511,7 +2508,7 @@
         <v>956.2808214978586</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="20">
         <v>50</v>
       </c>
@@ -2519,7 +2516,7 @@
         <v>972.64966236313182</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="20">
         <v>51</v>
       </c>
@@ -2527,7 +2524,7 @@
         <v>988.91325861156065</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="20">
         <v>52</v>
       </c>
@@ -2535,7 +2532,7 @@
         <v>1005.0726220070715</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="20">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Alt virkar sum tad skal nu uttan á MAC
</commit_message>
<xml_diff>
--- a/Opt_X.xlsx
+++ b/Opt_X.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rolvur Reinert\Desktop\P2X\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D635D562-FB52-4D55-9FA2-B5C5E3086996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAAE8E8-E703-4074-971C-2C0FA7E33B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AF05AB96-9D53-9746-847A-2DA4A160AAD8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="139">
   <si>
     <t>First day of the simulation</t>
   </si>
@@ -442,16 +442,19 @@
     <t>S_Pu_max</t>
   </si>
   <si>
-    <t>2020-01-13 00:00</t>
-  </si>
-  <si>
-    <t>2020-02-02 23:59</t>
-  </si>
-  <si>
     <t>Weekly</t>
   </si>
   <si>
-    <t>2020-01-26 23:59</t>
+    <t>2020-06-01 00:00</t>
+  </si>
+  <si>
+    <t>2020-06-07 23:59</t>
+  </si>
+  <si>
+    <t>2020-05-04 00:00</t>
+  </si>
+  <si>
+    <t>2020-05-10 23:59</t>
   </si>
 </sst>
 </file>
@@ -958,7 +961,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -988,7 +991,7 @@
         <v>110</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>111</v>
@@ -999,7 +1002,7 @@
         <v>77</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1016,7 +1019,7 @@
         <v>78</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1033,7 +1036,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1050,7 +1053,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -1067,7 +1070,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>

</xml_diff>